<commit_message>
Correção em estratégias e criação de novas
</commit_message>
<xml_diff>
--- a/extracteds/Cases/Execução/Extracted Venda em Horários - Quarta.xlsx
+++ b/extracteds/Cases/Execução/Extracted Venda em Horários - Quarta.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>Ativo</t>
   </si>
@@ -120,7 +120,7 @@
     <t>10:20</t>
   </si>
   <si>
-    <t xml:space="preserve">2021-12-29 10:05:00</t>
+    <t xml:space="preserve">2022-07-06 10:00:00</t>
   </si>
   <si>
     <t xml:space="preserve">2022-01-05 10:00:00</t>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>10:0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-12-29 10:05:00</t>
   </si>
   <si>
     <t>SIMH3</t>
@@ -223,7 +226,7 @@
     </font>
     <font>
       <name val="Calibri"/>
-      <color theme="9" tint="-0.249977111117893"/>
+      <color indexed="2"/>
       <sz val="11.000000"/>
       <scheme val="minor"/>
     </font>
@@ -264,12 +267,13 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="2" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="9" xfId="1" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="10" xfId="1" applyNumberFormat="1"/>
     <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="3" borderId="0" numFmtId="10" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf fontId="1" fillId="3" borderId="0" numFmtId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="4" borderId="0" numFmtId="10" xfId="1" applyNumberFormat="1" applyFill="1"/>
@@ -708,8 +712,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="6" max="10" style="1" width="9.140625"/>
-    <col bestFit="1" min="14" max="14" width="9.7109375"/>
+    <col customWidth="1" min="1" max="5" width="9.140625"/>
+    <col customWidth="1" min="6" max="10" style="1" width="9.140625"/>
+    <col customWidth="1" min="11" max="11" width="12.421875"/>
+    <col customWidth="1" min="12" max="13" width="9.140625"/>
+    <col bestFit="1" customWidth="1" min="14" max="14" width="9.7109375"/>
+    <col customWidth="1" min="15" max="16" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1104,7 +1112,7 @@
       <c r="I9" s="4">
         <v>-4.6106557377049162e-003</v>
       </c>
-      <c r="J9" s="4">
+      <c r="J9" s="5">
         <v>8.9999999999999993e-003</v>
       </c>
       <c r="K9" s="3" t="s">
@@ -1122,55 +1130,55 @@
       <c r="O9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="P9" s="5"/>
+      <c r="P9" s="6"/>
     </row>
     <row r="10">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="6">
-        <v>133</v>
-      </c>
-      <c r="C10" s="6">
-        <v>26</v>
-      </c>
-      <c r="D10" s="6">
-        <v>24</v>
-      </c>
-      <c r="E10" s="6">
-        <v>2</v>
-      </c>
-      <c r="F10" s="7">
-        <v>0.92307692307692313</v>
-      </c>
-      <c r="G10" s="7">
-        <v>0.26469546597711224</v>
-      </c>
-      <c r="H10" s="7">
-        <v>1.0180594845273548e-002</v>
-      </c>
-      <c r="I10" s="7">
-        <v>-6.9708491761723002e-003</v>
-      </c>
-      <c r="J10" s="8">
+      <c r="B10" s="7">
+        <v>146</v>
+      </c>
+      <c r="C10" s="7">
+        <v>29</v>
+      </c>
+      <c r="D10" s="7">
+        <v>25</v>
+      </c>
+      <c r="E10" s="7">
+        <v>4</v>
+      </c>
+      <c r="F10" s="8">
+        <v>0.86206896551724133</v>
+      </c>
+      <c r="G10" s="8">
+        <v>0.26301513339419724</v>
+      </c>
+      <c r="H10" s="8">
+        <v>9.0694873584205946e-003</v>
+      </c>
+      <c r="I10" s="8">
+        <v>-1.1293179805137221e-002</v>
+      </c>
+      <c r="J10" s="9">
         <v>1.2e-002</v>
       </c>
-      <c r="K10" s="6" t="s">
+      <c r="K10" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="L10" s="6" t="s">
+      <c r="L10" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="M10" s="6">
+      <c r="M10" s="7">
         <v>741300</v>
       </c>
-      <c r="N10" s="6">
-        <v>3687968.4210526315</v>
-      </c>
-      <c r="O10" s="6" t="s">
+      <c r="N10" s="7">
+        <v>3661512.3287671232</v>
+      </c>
+      <c r="O10" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="P10" s="6"/>
+      <c r="P10" s="7"/>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
@@ -1200,7 +1208,7 @@
       <c r="I11" s="4">
         <v>-5.5826936496859991e-003</v>
       </c>
-      <c r="J11" s="4">
+      <c r="J11" s="5">
         <v>8.9999999999999993e-003</v>
       </c>
       <c r="K11" s="3" t="s">
@@ -1346,7 +1354,7 @@
         <v>8.9999999999999993e-003</v>
       </c>
       <c r="K14" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="L14" t="s">
         <v>23</v>
@@ -1363,7 +1371,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B15">
         <v>133</v>
@@ -1393,7 +1401,7 @@
         <v>8.9999999999999993e-003</v>
       </c>
       <c r="K15" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L15" t="s">
         <v>23</v>
@@ -1440,7 +1448,7 @@
         <v>8.9999999999999993e-003</v>
       </c>
       <c r="K16" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="L16" t="s">
         <v>23</v>
@@ -1452,12 +1460,12 @@
         <v>3687968.4210526315</v>
       </c>
       <c r="O16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B17">
         <v>133</v>
@@ -1504,7 +1512,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B18">
         <v>133</v>
@@ -1534,10 +1542,10 @@
         <v>8.9999999999999993e-003</v>
       </c>
       <c r="K18" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="L18" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M18">
         <v>1515900</v>
@@ -1546,7 +1554,7 @@
         <v>9464527.8195488714</v>
       </c>
       <c r="O18" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19">
@@ -1598,7 +1606,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B20">
         <v>133</v>
@@ -1628,7 +1636,7 @@
         <v>8.9999999999999993e-003</v>
       </c>
       <c r="K20" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L20" t="s">
         <v>23</v>
@@ -1640,12 +1648,12 @@
         <v>12636709.022556391</v>
       </c>
       <c r="O20" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B21">
         <v>133</v>
@@ -1675,10 +1683,10 @@
         <v>8.9999999999999993e-003</v>
       </c>
       <c r="K21" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L21" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M21">
         <v>1515900</v>
@@ -1692,7 +1700,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B22">
         <v>133</v>
@@ -1725,7 +1733,7 @@
         <v>32</v>
       </c>
       <c r="L22" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="M22">
         <v>1515900</v>
@@ -1739,7 +1747,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B23">
         <v>133</v>
@@ -1769,7 +1777,7 @@
         <v>8.9999999999999993e-003</v>
       </c>
       <c r="K23" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L23" t="s">
         <v>23</v>
@@ -1786,7 +1794,7 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B24">
         <v>141</v>
@@ -1828,12 +1836,12 @@
         <v>1012276.5957446808</v>
       </c>
       <c r="O24" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B25">
         <v>141</v>
@@ -1863,10 +1871,10 @@
         <v>8.9999999999999993e-003</v>
       </c>
       <c r="K25" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L25" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="M25">
         <v>232200</v>
@@ -1875,12 +1883,12 @@
         <v>1292267.3758865248</v>
       </c>
       <c r="O25" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B26">
         <v>133</v>
@@ -1910,7 +1918,7 @@
         <v>8.9999999999999993e-003</v>
       </c>
       <c r="K26" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L26" t="s">
         <v>23</v>
@@ -1927,7 +1935,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B27">
         <v>133</v>
@@ -1974,7 +1982,7 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B28">
         <v>133</v>
@@ -2004,7 +2012,7 @@
         <v>8.9999999999999993e-003</v>
       </c>
       <c r="K28" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L28" t="s">
         <v>23</v>
@@ -11181,7 +11189,7 @@
   </sortState>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483647" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>